<commit_message>
mac Mie  2 Noi 2022 07:07:44 EET
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>571460</v>
+        <v>581024</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1050,7 +1050,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="4">
-        <v>573851</v>
+        <v>583415</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
mac Mie  2 Noi 2022 16:46:42 EET
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>581024</v>
+        <v>588197</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1050,7 +1050,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="4">
-        <v>583415</v>
+        <v>590588</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
mac Mie  2 Noi 2022 17:36:11 EET
</commit_message>
<xml_diff>
--- a/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
+++ b/SCRATCH/RELEASE/foaie_parcurs_B-151-VGT_octombrie_2022_Alex_Bora.xlsx
@@ -626,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>588197</v>
+        <v>590588</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -1050,7 +1050,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="4">
-        <v>590588</v>
+        <v>592979</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">

</xml_diff>